<commit_message>
update on PA Data
</commit_message>
<xml_diff>
--- a/Vale/Docs/DataPA/PA_Summary_2021.xlsx
+++ b/Vale/Docs/DataPA/PA_Summary_2021.xlsx
@@ -17,8 +17,6 @@
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName function="false" hidden="false" name="aclbseadj" vbProcedure="false">[6]Data!$FL$6:$FL$57</definedName>
@@ -29,14 +27,9 @@
     <definedName function="false" hidden="false" name="bucket" vbProcedure="false">[7]lookup!$A$3:$F$18</definedName>
     <definedName function="false" hidden="false" name="Bucket_Slag375" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Bunching_factor" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="calcine" vbProcedure="false">[8]lookup!$A$3:$B$8</definedName>
-    <definedName function="false" hidden="false" name="calcine1" vbProcedure="false">[8]lookup!$A$3:$B$8</definedName>
-    <definedName function="false" hidden="false" name="CAT375_BH_digging_rate" vbProcedure="false">[9]assumptions!#ref!</definedName>
     <definedName function="false" hidden="false" name="CAT375_rate" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="CAT5130_BH_digging_rate" vbProcedure="false">[9]assumptions!#ref!</definedName>
     <definedName function="false" hidden="false" name="CAT5130_rom_rate" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="CAT5130_strip_rate" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="CDB_EWH" vbProcedure="false">'[10]Wk_Press data'!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" name="CD_Fcast" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Chart" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Chart01" vbProcedure="false">#REF!</definedName>
@@ -391,8 +384,6 @@
     <definedName function="false" hidden="false" name="TruckF_Slag" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="TruckF_SlagPetea" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Truck_change_time" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Truck_Factor_777_OB" vbProcedure="false">[9]assumptions!#ref!</definedName>
-    <definedName function="false" hidden="false" name="Truck_Factor_777_ROM" vbProcedure="false">[9]assumptions!#ref!</definedName>
     <definedName function="false" hidden="false" name="truck_shortage" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="unit_cost" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="VARIANCE" vbProcedure="false">#REF!</definedName>
@@ -403,7 +394,6 @@
     <definedName function="false" hidden="false" name="WB_DKP_Rec" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="WB_DKP_RoM_Rec" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="WB_oredig_difficulty_factor" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Weekly_Report" vbProcedure="false">'[10]Wk_Press data'!$A$2:$K$406</definedName>
     <definedName function="false" hidden="false" name="WEST_2010" vbProcedure="false">Dryer_Balance</definedName>
     <definedName function="false" hidden="false" name="WF" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="wkmth" vbProcedure="false">[6]Data!$F$6:$F$57</definedName>
@@ -2539,7 +2529,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="191">
   <si>
     <t xml:space="preserve">Unit</t>
   </si>
@@ -3084,7 +3074,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Shutted off</t>
+    <t xml:space="preserve">Shutted Off</t>
   </si>
   <si>
     <t xml:space="preserve">CW-117 Relief Valve</t>
@@ -3189,7 +3179,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Total Black Out</t>
+    <t xml:space="preserve">Total Blackout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment Trip</t>
   </si>
   <si>
     <t xml:space="preserve">A1G1 </t>
@@ -3755,65 +3748,78 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="PARAMETER"/>
-      <sheetName val="Summary_Gab"/>
-      <sheetName val="SUMMARY "/>
-      <sheetName val="Plan Monthly"/>
-      <sheetName val="Summary by Hill"/>
-      <sheetName val="West_Yearly"/>
-      <sheetName val="West 1st Half"/>
-      <sheetName val="West 2nd Half"/>
-      <sheetName val="DATA_XXX"/>
-      <sheetName val="Petea_Yearly"/>
-      <sheetName val="Petea_1st Half"/>
-      <sheetName val="Petea_2nd Half"/>
-      <sheetName val="Production Summary"/>
-      <sheetName val="Chart-OB"/>
-      <sheetName val="Chart-ROM"/>
-      <sheetName val="Chart-SSP"/>
-      <sheetName val="Chart-OB(W) Distribution"/>
-      <sheetName val="Chart-OB(E) Distribution"/>
-      <sheetName val="Chart-ROM (W) Distribution"/>
-      <sheetName val="Chart-ROM (E) Distribution"/>
-      <sheetName val="Monthly_Ni"/>
-      <sheetName val="Monthly_Fe"/>
-      <sheetName val="Monthly_SM"/>
-      <sheetName val="Monthly_Co"/>
-      <sheetName val="Monthly_SR"/>
-      <sheetName val="Monthly_Civil"/>
-      <sheetName val="Monthly_DKP Prod"/>
-      <sheetName val="Monthly_WOS Stat"/>
-      <sheetName val="Monthly_LBS Ni"/>
-      <sheetName val="OB_Distance"/>
-      <sheetName val="ROM_Distance"/>
-      <sheetName val="SSP_Distance"/>
-      <sheetName val="Quarry_Distance"/>
-      <sheetName val="SS#5_Prod"/>
-      <sheetName val="SS#8_Prod"/>
-      <sheetName val="SS#9_Prod"/>
-      <sheetName val="SS#11_Prod"/>
-      <sheetName val="SS#10_Pet"/>
-      <sheetName val="SS#All"/>
-      <sheetName val="Ni_Grade"/>
-      <sheetName val="Fe_Grade"/>
-      <sheetName val="SM_Ratio"/>
-      <sheetName val="Chart-OB by Hill"/>
-      <sheetName val="Chart-ROM by Hill"/>
-      <sheetName val="Chart-Civil by Hill"/>
-      <sheetName val="Chart-SSP by Hill"/>
-      <sheetName val="Chart-OREX by Hill"/>
-      <sheetName val="Chart-DKP by Hill"/>
-      <sheetName val="Chart-lbs by hill"/>
-      <sheetName val="Update_Data"/>
-      <sheetName val="%Op_time"/>
-      <sheetName val="EF1_Data"/>
-      <sheetName val="Pow_Set"/>
-      <sheetName val="EF2_Data"/>
-      <sheetName val="Avg_Pow"/>
-      <sheetName val="EF3_Data"/>
-      <sheetName val="Calcine"/>
-      <sheetName val="EF4_Data"/>
-      <sheetName val="EFT_Data"/>
+      <sheetName val="Assumptions"/>
+      <sheetName val="Blend Options"/>
+      <sheetName val="Screening Stations"/>
+      <sheetName val="Calcine Options"/>
+      <sheetName val="EF#1"/>
+      <sheetName val="RK#1"/>
+      <sheetName val="Blend_Options"/>
+      <sheetName val="Screening_Stations"/>
+      <sheetName val="Calcine_Options"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="rev"/>
+      <sheetName val="actual"/>
+      <sheetName val="actual-M"/>
+      <sheetName val="chart"/>
+      <sheetName val="Map"/>
+      <sheetName val="Grade Calculator (2)"/>
+      <sheetName val="CCP2-2Y"/>
+      <sheetName val="historical"/>
+      <sheetName val="Shutdown"/>
+      <sheetName val="Major Shutdown"/>
+      <sheetName val="Reforcast"/>
+      <sheetName val="cpanel"/>
+      <sheetName val="summary"/>
+      <sheetName val="monthly"/>
+      <sheetName val="weekly"/>
+      <sheetName val="bulk-chart"/>
+      <sheetName val="bulk"/>
+      <sheetName val="shipment"/>
+      <sheetName val="oee"/>
+      <sheetName val="2015"/>
+      <sheetName val="2016"/>
+      <sheetName val="Master Schedule"/>
+      <sheetName val="2017"/>
+      <sheetName val="OD OF Historical"/>
+      <sheetName val="EF OF Historical"/>
+      <sheetName val="RK OF Historical"/>
+      <sheetName val="CV OF Historical"/>
+      <sheetName val="Balance"/>
+      <sheetName val="2015Mine"/>
+      <sheetName val="2016Mine"/>
+      <sheetName val="2016Mine-Ori"/>
+      <sheetName val="2017Mine"/>
+      <sheetName val="2017Mine-Ori"/>
+      <sheetName val="Individual"/>
+      <sheetName val="Operating Data"/>
+      <sheetName val="Process Variables"/>
+      <sheetName val="Inv &amp; Comp"/>
+      <sheetName val="Equipment &amp; Dashboard"/>
+      <sheetName val="CCP2-6M"/>
+      <sheetName val="Grade Calculator"/>
+      <sheetName val="check mine"/>
+      <sheetName val="MP_Inv"/>
+      <sheetName val="Scrap_Inv"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -3859,28 +3865,12 @@
       <sheetData sheetId="40"/>
       <sheetData sheetId="41"/>
       <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3917,7 +3907,28 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="PM Schedule Revisi 3"/>
+      <sheetName val="Availability"/>
+      <sheetName val="Compliance"/>
+      <sheetName val="Revision History"/>
+      <sheetName val="lookup"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4242,282 +4253,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Contents"/>
-      <sheetName val="Dashboard"/>
-      <sheetName val="KPIs"/>
-      <sheetName val="Annual Operating Costs"/>
-      <sheetName val="Op Costs by area"/>
-      <sheetName val="1. Financial forecasts"/>
-      <sheetName val="Profit and loss"/>
-      <sheetName val="Cash flow"/>
-      <sheetName val="Balance sheet"/>
-      <sheetName val="Reserves"/>
-      <sheetName val="1.B. CAR Tabs"/>
-      <sheetName val="Notes"/>
-      <sheetName val="Charts"/>
-      <sheetName val="Scen Comp (2006)"/>
-      <sheetName val="Scen Comp (2004)"/>
-      <sheetName val="Tables and Results"/>
-      <sheetName val="2. Inputs"/>
-      <sheetName val="Control and Sensitivity"/>
-      <sheetName val="Prices"/>
-      <sheetName val="Mining case inputs"/>
-      <sheetName val="Process inputs"/>
-      <sheetName val="Utilities inputs"/>
-      <sheetName val="Corp Expense inputs"/>
-      <sheetName val="Capital expenditure inputs"/>
-      <sheetName val="Other inputs"/>
-      <sheetName val="Reserve inputs"/>
-      <sheetName val="Balance sheet inputs"/>
-      <sheetName val="3. Mining"/>
-      <sheetName val="DKP production"/>
-      <sheetName val="Mining Costs"/>
-      <sheetName val="4. Process"/>
-      <sheetName val="Nickel in matte production"/>
-      <sheetName val="Process Plant Costs"/>
-      <sheetName val="5. Utilities"/>
-      <sheetName val="Utilities production"/>
-      <sheetName val="Utilities costs"/>
-      <sheetName val="6. Capex &amp; other"/>
-      <sheetName val="Capex"/>
-      <sheetName val="Working Cap"/>
-      <sheetName val="Lease schedule"/>
-      <sheetName val="Other expenses"/>
-      <sheetName val="Rupiah impact"/>
-      <sheetName val="7. Tax"/>
-      <sheetName val="Tax"/>
-      <sheetName val="Indirect taxes &amp; royalties"/>
-      <sheetName val="Accounting depreciation"/>
-      <sheetName val="Tax depreciation prior to 2008"/>
-      <sheetName val="Tax depreciation post 2008"/>
-      <sheetName val="KHP Tax depreciation"/>
-      <sheetName val="Appendix"/>
-      <sheetName val="Chart data"/>
-      <sheetName val="Data validation"/>
-      <sheetName val="Names"/>
-      <sheetName val="Workbook key"/>
-      <sheetName val="Energy"/>
-      <sheetName val="52 wks rolling data"/>
-      <sheetName val="Production"/>
-      <sheetName val="Generator"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PM Schedule Revisi 3"/>
-      <sheetName val="Availability"/>
-      <sheetName val="Compliance"/>
-      <sheetName val="Revision History"/>
-      <sheetName val="lookup"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Assumptions"/>
-      <sheetName val="Blend Options"/>
-      <sheetName val="Screening Stations"/>
-      <sheetName val="Calcine Options"/>
-      <sheetName val="EF#1"/>
-      <sheetName val="RK#1"/>
-      <sheetName val="Blend_Options"/>
-      <sheetName val="Screening_Stations"/>
-      <sheetName val="Calcine_Options"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="rev"/>
-      <sheetName val="actual"/>
-      <sheetName val="actual-M"/>
-      <sheetName val="chart"/>
-      <sheetName val="Map"/>
-      <sheetName val="Grade Calculator (2)"/>
-      <sheetName val="CCP2-2Y"/>
-      <sheetName val="historical"/>
-      <sheetName val="Shutdown"/>
-      <sheetName val="Major Shutdown"/>
-      <sheetName val="Reforcast"/>
-      <sheetName val="cpanel"/>
-      <sheetName val="summary"/>
-      <sheetName val="monthly"/>
-      <sheetName val="weekly"/>
-      <sheetName val="bulk-chart"/>
-      <sheetName val="bulk"/>
-      <sheetName val="shipment"/>
-      <sheetName val="oee"/>
-      <sheetName val="2015"/>
-      <sheetName val="2016"/>
-      <sheetName val="Master Schedule"/>
-      <sheetName val="2017"/>
-      <sheetName val="OD OF Historical"/>
-      <sheetName val="EF OF Historical"/>
-      <sheetName val="RK OF Historical"/>
-      <sheetName val="CV OF Historical"/>
-      <sheetName val="Balance"/>
-      <sheetName val="2015Mine"/>
-      <sheetName val="2016Mine"/>
-      <sheetName val="2016Mine-Ori"/>
-      <sheetName val="2017Mine"/>
-      <sheetName val="2017Mine-Ori"/>
-      <sheetName val="Individual"/>
-      <sheetName val="Operating Data"/>
-      <sheetName val="Process Variables"/>
-      <sheetName val="Inv &amp; Comp"/>
-      <sheetName val="Equipment &amp; Dashboard"/>
-      <sheetName val="CCP2-6M"/>
-      <sheetName val="Grade Calculator"/>
-      <sheetName val="check mine"/>
-      <sheetName val="MP_Inv"/>
-      <sheetName val="Scrap_Inv"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
@@ -27431,10 +27166,10 @@
   </sheetPr>
   <dimension ref="A1:V366"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="R3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U14" activeCellId="0" sqref="U14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="R149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="S167" activeCellId="0" sqref="S167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -46346,13 +46081,13 @@
         <v>104</v>
       </c>
       <c r="S337" s="32" t="s">
-        <v>117</v>
+        <v>187</v>
       </c>
       <c r="T337" s="32" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U337" s="32" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46988,7 +46723,7 @@
         <v>0</v>
       </c>
       <c r="Q349" s="41" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R349" s="32" t="s">
         <v>104</v>

</xml_diff>